<commit_message>
adding xl practice data
</commit_message>
<xml_diff>
--- a/docs/assets/data/xlexamples/nea_grants.xlsx
+++ b/docs/assets/data/xlexamples/nea_grants.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shcohen1/Documents/GitHub/cronkite-docs/docs/assets/data/xlexamples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B332276-BD71-BA42-9B74-745F817582EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A5CBB4-3557-494E-9352-733CD5CD4200}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="21560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grants" sheetId="1" r:id="rId1"/>
     <sheet name="source" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Grants!$A$1:$N$520</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4688" uniqueCount="1386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4689" uniqueCount="1387">
   <si>
     <t>Organization Name</t>
   </si>
@@ -4178,7 +4181,10 @@
     <t>https://apps.nea.gov/grantsearch/</t>
   </si>
   <si>
-    <t xml:space="preserve">although when I went to it just now, it has an error and you can't search it. </t>
+    <t>javascript:openFaq()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is an FAQ link that does some </t>
   </si>
 </sst>
 </file>
@@ -4555,14 +4561,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N520"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
+      <selection activeCell="L349" sqref="L349"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="2" max="2" width="47.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="37" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
@@ -4576,7 +4582,7 @@
     <col min="14" max="14" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" ht="16">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4620,7 +4626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4664,7 +4670,7 @@
         <v>37590</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4708,7 +4714,7 @@
         <v>36891</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -4752,7 +4758,7 @@
         <v>37376</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4796,7 +4802,7 @@
         <v>36891</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -4840,7 +4846,7 @@
         <v>37925</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -4884,7 +4890,7 @@
         <v>37164</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -4928,7 +4934,7 @@
         <v>37437</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -4972,7 +4978,7 @@
         <v>37164</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -5016,7 +5022,7 @@
         <v>36922</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -5060,7 +5066,7 @@
         <v>37376</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -5104,7 +5110,7 @@
         <v>37287</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -5148,7 +5154,7 @@
         <v>36981</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -5192,7 +5198,7 @@
         <v>37164</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -5236,7 +5242,7 @@
         <v>37225</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -5280,7 +5286,7 @@
         <v>37164</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -5324,7 +5330,7 @@
         <v>37134</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -5368,7 +5374,7 @@
         <v>37134</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -5412,7 +5418,7 @@
         <v>37437</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -5456,7 +5462,7 @@
         <v>37376</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -5500,7 +5506,7 @@
         <v>36950</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15">
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -5544,7 +5550,7 @@
         <v>37256</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15">
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -5588,7 +5594,7 @@
         <v>37256</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15">
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -5632,7 +5638,7 @@
         <v>37802</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15">
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -5676,7 +5682,7 @@
         <v>37407</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -5720,7 +5726,7 @@
         <v>37195</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -5764,7 +5770,7 @@
         <v>37529</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15">
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -5808,7 +5814,7 @@
         <v>37864</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15">
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>126</v>
       </c>
@@ -5852,7 +5858,7 @@
         <v>38717</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15">
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -5896,7 +5902,7 @@
         <v>37529</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -5940,7 +5946,7 @@
         <v>37072</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -5984,7 +5990,7 @@
         <v>37315</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15">
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -6028,7 +6034,7 @@
         <v>37652</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15">
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -6072,7 +6078,7 @@
         <v>37072</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>146</v>
       </c>
@@ -6116,7 +6122,7 @@
         <v>37407</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15">
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>152</v>
       </c>
@@ -6160,7 +6166,7 @@
         <v>37499</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15">
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -6204,7 +6210,7 @@
         <v>37529</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -6248,7 +6254,7 @@
         <v>37437</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -6292,7 +6298,7 @@
         <v>37529</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -6336,7 +6342,7 @@
         <v>37711</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -6380,7 +6386,7 @@
         <v>37437</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -6424,7 +6430,7 @@
         <v>39355</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -6468,7 +6474,7 @@
         <v>37499</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15">
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -6512,7 +6518,7 @@
         <v>37621</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15">
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>181</v>
       </c>
@@ -6556,7 +6562,7 @@
         <v>37499</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15">
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>185</v>
       </c>
@@ -6600,7 +6606,7 @@
         <v>37407</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15">
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>191</v>
       </c>
@@ -6644,7 +6650,7 @@
         <v>37407</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15">
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -6688,7 +6694,7 @@
         <v>37407</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15">
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -6732,7 +6738,7 @@
         <v>37802</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -6776,7 +6782,7 @@
         <v>37802</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -6820,7 +6826,7 @@
         <v>37376</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15">
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -6864,7 +6870,7 @@
         <v>37621</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15">
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -6908,7 +6914,7 @@
         <v>38168</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="15">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -6952,7 +6958,7 @@
         <v>37407</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="15">
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>45</v>
       </c>
@@ -6996,7 +7002,7 @@
         <v>37894</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="15">
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -7040,7 +7046,7 @@
         <v>37802</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="15">
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>213</v>
       </c>
@@ -7084,7 +7090,7 @@
         <v>38230</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="15">
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -7128,7 +7134,7 @@
         <v>37894</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="15">
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -7172,7 +7178,7 @@
         <v>37560</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="15">
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>220</v>
       </c>
@@ -7216,7 +7222,7 @@
         <v>37864</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="15">
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
         <v>141</v>
       </c>
@@ -7260,7 +7266,7 @@
         <v>38046</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="15">
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>226</v>
       </c>
@@ -7304,7 +7310,7 @@
         <v>37772</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="15">
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
         <v>230</v>
       </c>
@@ -7348,7 +7354,7 @@
         <v>38168</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15">
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
         <v>94</v>
       </c>
@@ -7392,7 +7398,7 @@
         <v>38168</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15">
+    <row r="65" spans="1:14">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -7436,7 +7442,7 @@
         <v>38168</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15">
+    <row r="66" spans="1:14">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -7480,7 +7486,7 @@
         <v>37986</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15">
+    <row r="67" spans="1:14">
       <c r="A67" t="s">
         <v>45</v>
       </c>
@@ -7524,7 +7530,7 @@
         <v>38383</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="15">
+    <row r="68" spans="1:14">
       <c r="A68" t="s">
         <v>36</v>
       </c>
@@ -7568,7 +7574,7 @@
         <v>38260</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15">
+    <row r="69" spans="1:14">
       <c r="A69" t="s">
         <v>230</v>
       </c>
@@ -7612,7 +7618,7 @@
         <v>37986</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15">
+    <row r="70" spans="1:14">
       <c r="A70" t="s">
         <v>45</v>
       </c>
@@ -7656,7 +7662,7 @@
         <v>38533</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15">
+    <row r="71" spans="1:14">
       <c r="A71" t="s">
         <v>191</v>
       </c>
@@ -7700,7 +7706,7 @@
         <v>38168</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15">
+    <row r="72" spans="1:14">
       <c r="A72" t="s">
         <v>255</v>
       </c>
@@ -7744,7 +7750,7 @@
         <v>38595</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15">
+    <row r="73" spans="1:14">
       <c r="A73" t="s">
         <v>260</v>
       </c>
@@ -7788,7 +7794,7 @@
         <v>38291</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15">
+    <row r="74" spans="1:14">
       <c r="A74" t="s">
         <v>264</v>
       </c>
@@ -7832,7 +7838,7 @@
         <v>38564</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15">
+    <row r="75" spans="1:14">
       <c r="A75" t="s">
         <v>70</v>
       </c>
@@ -7876,7 +7882,7 @@
         <v>39355</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15">
+    <row r="76" spans="1:14">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -7920,7 +7926,7 @@
         <v>38260</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="15">
+    <row r="77" spans="1:14">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -7964,7 +7970,7 @@
         <v>38533</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15">
+    <row r="78" spans="1:14">
       <c r="A78" t="s">
         <v>94</v>
       </c>
@@ -8008,7 +8014,7 @@
         <v>38533</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="15">
+    <row r="79" spans="1:14">
       <c r="A79" t="s">
         <v>275</v>
       </c>
@@ -8052,7 +8058,7 @@
         <v>38383</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="15">
+    <row r="80" spans="1:14">
       <c r="A80" t="s">
         <v>279</v>
       </c>
@@ -8096,7 +8102,7 @@
         <v>38533</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="15">
+    <row r="81" spans="1:14">
       <c r="A81" t="s">
         <v>255</v>
       </c>
@@ -8140,7 +8146,7 @@
         <v>38503</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="15">
+    <row r="82" spans="1:14">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -8184,7 +8190,7 @@
         <v>38138</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="15">
+    <row r="83" spans="1:14">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -8228,7 +8234,7 @@
         <v>38868</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="15">
+    <row r="84" spans="1:14">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -8272,7 +8278,7 @@
         <v>38472</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="15">
+    <row r="85" spans="1:14">
       <c r="A85" t="s">
         <v>23</v>
       </c>
@@ -8316,7 +8322,7 @@
         <v>38321</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="15">
+    <row r="86" spans="1:14">
       <c r="A86" t="s">
         <v>36</v>
       </c>
@@ -8360,7 +8366,7 @@
         <v>38168</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="15">
+    <row r="87" spans="1:14">
       <c r="A87" t="s">
         <v>113</v>
       </c>
@@ -8404,7 +8410,7 @@
         <v>38291</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="15">
+    <row r="88" spans="1:14">
       <c r="A88" t="s">
         <v>113</v>
       </c>
@@ -8448,7 +8454,7 @@
         <v>38472</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="15">
+    <row r="89" spans="1:14">
       <c r="A89" t="s">
         <v>300</v>
       </c>
@@ -8492,7 +8498,7 @@
         <v>38868</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="15">
+    <row r="90" spans="1:14">
       <c r="A90" t="s">
         <v>305</v>
       </c>
@@ -8536,7 +8542,7 @@
         <v>38260</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="15">
+    <row r="91" spans="1:14">
       <c r="A91" t="s">
         <v>309</v>
       </c>
@@ -8580,7 +8586,7 @@
         <v>38503</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="15">
+    <row r="92" spans="1:14">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -8624,7 +8630,7 @@
         <v>38442</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="15">
+    <row r="93" spans="1:14">
       <c r="A93" t="s">
         <v>45</v>
       </c>
@@ -8668,7 +8674,7 @@
         <v>38503</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="15">
+    <row r="94" spans="1:14">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -8712,7 +8718,7 @@
         <v>38352</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="15">
+    <row r="95" spans="1:14">
       <c r="A95" t="s">
         <v>319</v>
       </c>
@@ -8756,7 +8762,7 @@
         <v>38656</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="15">
+    <row r="96" spans="1:14">
       <c r="A96" t="s">
         <v>220</v>
       </c>
@@ -8800,7 +8806,7 @@
         <v>38656</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="15">
+    <row r="97" spans="1:14">
       <c r="A97" t="s">
         <v>146</v>
       </c>
@@ -8844,7 +8850,7 @@
         <v>38503</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="15">
+    <row r="98" spans="1:14">
       <c r="A98" t="s">
         <v>70</v>
       </c>
@@ -8888,7 +8894,7 @@
         <v>38717</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="15">
+    <row r="99" spans="1:14">
       <c r="A99" t="s">
         <v>29</v>
       </c>
@@ -8932,7 +8938,7 @@
         <v>38138</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="15">
+    <row r="100" spans="1:14">
       <c r="A100" t="s">
         <v>88</v>
       </c>
@@ -8976,7 +8982,7 @@
         <v>38898</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="15">
+    <row r="101" spans="1:14">
       <c r="A101" t="s">
         <v>336</v>
       </c>
@@ -9020,7 +9026,7 @@
         <v>39416</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="15">
+    <row r="102" spans="1:14">
       <c r="A102" t="s">
         <v>94</v>
       </c>
@@ -9064,7 +9070,7 @@
         <v>38898</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="15">
+    <row r="103" spans="1:14">
       <c r="A103" t="s">
         <v>342</v>
       </c>
@@ -9108,7 +9114,7 @@
         <v>38717</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="15">
+    <row r="104" spans="1:14">
       <c r="A104" t="s">
         <v>346</v>
       </c>
@@ -9152,7 +9158,7 @@
         <v>38717</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="15">
+    <row r="105" spans="1:14">
       <c r="A105" t="s">
         <v>14</v>
       </c>
@@ -9196,7 +9202,7 @@
         <v>38807</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="15">
+    <row r="106" spans="1:14">
       <c r="A106" t="s">
         <v>36</v>
       </c>
@@ -9240,7 +9246,7 @@
         <v>38868</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="15">
+    <row r="107" spans="1:14">
       <c r="A107" t="s">
         <v>45</v>
       </c>
@@ -9284,7 +9290,7 @@
         <v>38960</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="15">
+    <row r="108" spans="1:14">
       <c r="A108" t="s">
         <v>359</v>
       </c>
@@ -9328,7 +9334,7 @@
         <v>39082</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="15">
+    <row r="109" spans="1:14">
       <c r="A109" t="s">
         <v>45</v>
       </c>
@@ -9372,7 +9378,7 @@
         <v>38472</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="15">
+    <row r="110" spans="1:14">
       <c r="A110" t="s">
         <v>230</v>
       </c>
@@ -9416,7 +9422,7 @@
         <v>38533</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="15">
+    <row r="111" spans="1:14">
       <c r="A111" t="s">
         <v>367</v>
       </c>
@@ -9460,7 +9466,7 @@
         <v>38898</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="15">
+    <row r="112" spans="1:14">
       <c r="A112" t="s">
         <v>371</v>
       </c>
@@ -9504,7 +9510,7 @@
         <v>38960</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="15">
+    <row r="113" spans="1:14">
       <c r="A113" t="s">
         <v>70</v>
       </c>
@@ -9548,7 +9554,7 @@
         <v>38990</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="15">
+    <row r="114" spans="1:14">
       <c r="A114" t="s">
         <v>52</v>
       </c>
@@ -9592,7 +9598,7 @@
         <v>38686</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="15">
+    <row r="115" spans="1:14">
       <c r="A115" t="s">
         <v>377</v>
       </c>
@@ -9636,7 +9642,7 @@
         <v>38807</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="15">
+    <row r="116" spans="1:14">
       <c r="A116" t="s">
         <v>382</v>
       </c>
@@ -9680,7 +9686,7 @@
         <v>38656</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="15">
+    <row r="117" spans="1:14">
       <c r="A117" t="s">
         <v>387</v>
       </c>
@@ -9724,7 +9730,7 @@
         <v>38472</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="15">
+    <row r="118" spans="1:14">
       <c r="A118" t="s">
         <v>275</v>
       </c>
@@ -9768,7 +9774,7 @@
         <v>38868</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="15">
+    <row r="119" spans="1:14">
       <c r="A119" t="s">
         <v>88</v>
       </c>
@@ -9812,7 +9818,7 @@
         <v>39263</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="15">
+    <row r="120" spans="1:14">
       <c r="A120" t="s">
         <v>94</v>
       </c>
@@ -9856,7 +9862,7 @@
         <v>39263</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="15">
+    <row r="121" spans="1:14">
       <c r="A121" t="s">
         <v>279</v>
       </c>
@@ -9900,7 +9906,7 @@
         <v>39202</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="15">
+    <row r="122" spans="1:14">
       <c r="A122" t="s">
         <v>14</v>
       </c>
@@ -9944,7 +9950,7 @@
         <v>38868</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="15">
+    <row r="123" spans="1:14">
       <c r="A123" t="s">
         <v>23</v>
       </c>
@@ -9988,7 +9994,7 @@
         <v>38898</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="15">
+    <row r="124" spans="1:14">
       <c r="A124" t="s">
         <v>387</v>
       </c>
@@ -10032,7 +10038,7 @@
         <v>38990</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="15">
+    <row r="125" spans="1:14">
       <c r="A125" t="s">
         <v>36</v>
       </c>
@@ -10076,7 +10082,7 @@
         <v>38898</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="15">
+    <row r="126" spans="1:14">
       <c r="A126" t="s">
         <v>230</v>
       </c>
@@ -10120,7 +10126,7 @@
         <v>39782</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="15">
+    <row r="127" spans="1:14">
       <c r="A127" t="s">
         <v>305</v>
       </c>
@@ -10164,7 +10170,7 @@
         <v>40117</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="15">
+    <row r="128" spans="1:14">
       <c r="A128" t="s">
         <v>45</v>
       </c>
@@ -10208,7 +10214,7 @@
         <v>40209</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="15">
+    <row r="129" spans="1:14">
       <c r="A129" t="s">
         <v>70</v>
       </c>
@@ -10252,7 +10258,7 @@
         <v>38868</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="15">
+    <row r="130" spans="1:14">
       <c r="A130" t="s">
         <v>418</v>
       </c>
@@ -10296,7 +10302,7 @@
         <v>39233</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="15">
+    <row r="131" spans="1:14">
       <c r="A131" t="s">
         <v>255</v>
       </c>
@@ -10340,7 +10346,7 @@
         <v>39233</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="15">
+    <row r="132" spans="1:14">
       <c r="A132" t="s">
         <v>426</v>
       </c>
@@ -10384,7 +10390,7 @@
         <v>39233</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="15">
+    <row r="133" spans="1:14">
       <c r="A133" t="s">
         <v>36</v>
       </c>
@@ -10428,7 +10434,7 @@
         <v>39263</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="15">
+    <row r="134" spans="1:14">
       <c r="A134" t="s">
         <v>45</v>
       </c>
@@ -10472,7 +10478,7 @@
         <v>39325</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="15">
+    <row r="135" spans="1:14">
       <c r="A135" t="s">
         <v>434</v>
       </c>
@@ -10516,7 +10522,7 @@
         <v>39263</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="15">
+    <row r="136" spans="1:14">
       <c r="A136" t="s">
         <v>45</v>
       </c>
@@ -10560,7 +10566,7 @@
         <v>39082</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="15">
+    <row r="137" spans="1:14">
       <c r="A137" t="s">
         <v>230</v>
       </c>
@@ -10604,7 +10610,7 @@
         <v>39051</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="15">
+    <row r="138" spans="1:14">
       <c r="A138" t="s">
         <v>52</v>
       </c>
@@ -10648,7 +10654,7 @@
         <v>39233</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="15">
+    <row r="139" spans="1:14">
       <c r="A139" t="s">
         <v>191</v>
       </c>
@@ -10692,7 +10698,7 @@
         <v>38837</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="15">
+    <row r="140" spans="1:14">
       <c r="A140" t="s">
         <v>70</v>
       </c>
@@ -10736,7 +10742,7 @@
         <v>39355</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="15">
+    <row r="141" spans="1:14">
       <c r="A141" t="s">
         <v>29</v>
       </c>
@@ -10780,7 +10786,7 @@
         <v>39447</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="15">
+    <row r="142" spans="1:14">
       <c r="A142" t="s">
         <v>36</v>
       </c>
@@ -10824,7 +10830,7 @@
         <v>39629</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="15">
+    <row r="143" spans="1:14">
       <c r="A143" t="s">
         <v>450</v>
       </c>
@@ -10868,7 +10874,7 @@
         <v>39021</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="15">
+    <row r="144" spans="1:14">
       <c r="A144" t="s">
         <v>45</v>
       </c>
@@ -10912,7 +10918,7 @@
         <v>38776</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="15">
+    <row r="145" spans="1:14">
       <c r="A145" t="s">
         <v>457</v>
       </c>
@@ -10956,7 +10962,7 @@
         <v>39294</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="15">
+    <row r="146" spans="1:14">
       <c r="A146" t="s">
         <v>14</v>
       </c>
@@ -11000,7 +11006,7 @@
         <v>39872</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="15">
+    <row r="147" spans="1:14">
       <c r="A147" t="s">
         <v>94</v>
       </c>
@@ -11044,7 +11050,7 @@
         <v>39629</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="15">
+    <row r="148" spans="1:14">
       <c r="A148" t="s">
         <v>336</v>
       </c>
@@ -11088,7 +11094,7 @@
         <v>39813</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="15">
+    <row r="149" spans="1:14">
       <c r="A149" t="s">
         <v>88</v>
       </c>
@@ -11132,7 +11138,7 @@
         <v>39629</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="15">
+    <row r="150" spans="1:14">
       <c r="A150" t="s">
         <v>23</v>
       </c>
@@ -11176,7 +11182,7 @@
         <v>39568</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="15">
+    <row r="151" spans="1:14">
       <c r="A151" t="s">
         <v>14</v>
       </c>
@@ -11220,7 +11226,7 @@
         <v>39599</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="15">
+    <row r="152" spans="1:14">
       <c r="A152" t="s">
         <v>387</v>
       </c>
@@ -11264,7 +11270,7 @@
         <v>39355</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="15">
+    <row r="153" spans="1:14">
       <c r="A153" t="s">
         <v>45</v>
       </c>
@@ -11308,7 +11314,7 @@
         <v>40056</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="15">
+    <row r="154" spans="1:14">
       <c r="A154" t="s">
         <v>230</v>
       </c>
@@ -11352,7 +11358,7 @@
         <v>39599</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="15">
+    <row r="155" spans="1:14">
       <c r="A155" t="s">
         <v>305</v>
       </c>
@@ -11396,7 +11402,7 @@
         <v>39994</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="15">
+    <row r="156" spans="1:14">
       <c r="A156" t="s">
         <v>45</v>
       </c>
@@ -11440,7 +11446,7 @@
         <v>39507</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="15">
+    <row r="157" spans="1:14">
       <c r="A157" t="s">
         <v>36</v>
       </c>
@@ -11484,7 +11490,7 @@
         <v>39629</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="15">
+    <row r="158" spans="1:14">
       <c r="A158" t="s">
         <v>486</v>
       </c>
@@ -11528,7 +11534,7 @@
         <v>39447</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="15">
+    <row r="159" spans="1:14">
       <c r="A159" t="s">
         <v>489</v>
       </c>
@@ -11572,7 +11578,7 @@
         <v>39386</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="15">
+    <row r="160" spans="1:14">
       <c r="A160" t="s">
         <v>495</v>
       </c>
@@ -11616,7 +11622,7 @@
         <v>39386</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="15">
+    <row r="161" spans="1:14">
       <c r="A161" t="s">
         <v>45</v>
       </c>
@@ -11660,7 +11666,7 @@
         <v>39447</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="15">
+    <row r="162" spans="1:14">
       <c r="A162" t="s">
         <v>230</v>
       </c>
@@ -11704,7 +11710,7 @@
         <v>39263</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="15">
+    <row r="163" spans="1:14">
       <c r="A163" t="s">
         <v>70</v>
       </c>
@@ -11748,7 +11754,7 @@
         <v>39721</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="15">
+    <row r="164" spans="1:14">
       <c r="A164" t="s">
         <v>505</v>
       </c>
@@ -11792,7 +11798,7 @@
         <v>39721</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="15">
+    <row r="165" spans="1:14">
       <c r="A165" t="s">
         <v>450</v>
       </c>
@@ -11836,7 +11842,7 @@
         <v>39721</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="15">
+    <row r="166" spans="1:14">
       <c r="A166" t="s">
         <v>513</v>
       </c>
@@ -11880,7 +11886,7 @@
         <v>39386</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="15">
+    <row r="167" spans="1:14">
       <c r="A167" t="s">
         <v>518</v>
       </c>
@@ -11924,7 +11930,7 @@
         <v>39933</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="15">
+    <row r="168" spans="1:14">
       <c r="A168" t="s">
         <v>522</v>
       </c>
@@ -11968,7 +11974,7 @@
         <v>39507</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="15">
+    <row r="169" spans="1:14">
       <c r="A169" t="s">
         <v>528</v>
       </c>
@@ -12012,7 +12018,7 @@
         <v>39507</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="15">
+    <row r="170" spans="1:14">
       <c r="A170" t="s">
         <v>532</v>
       </c>
@@ -12056,7 +12062,7 @@
         <v>40086</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="15">
+    <row r="171" spans="1:14">
       <c r="A171" t="s">
         <v>537</v>
       </c>
@@ -12100,7 +12106,7 @@
         <v>39994</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="15">
+    <row r="172" spans="1:14">
       <c r="A172" t="s">
         <v>14</v>
       </c>
@@ -12144,7 +12150,7 @@
         <v>39629</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="15">
+    <row r="173" spans="1:14">
       <c r="A173" t="s">
         <v>23</v>
       </c>
@@ -12188,7 +12194,7 @@
         <v>39660</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="15">
+    <row r="174" spans="1:14">
       <c r="A174" t="s">
         <v>387</v>
       </c>
@@ -12232,7 +12238,7 @@
         <v>39721</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="15">
+    <row r="175" spans="1:14">
       <c r="A175" t="s">
         <v>36</v>
       </c>
@@ -12276,7 +12282,7 @@
         <v>40421</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="15">
+    <row r="176" spans="1:14">
       <c r="A176" t="s">
         <v>309</v>
       </c>
@@ -12320,7 +12326,7 @@
         <v>39994</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="15">
+    <row r="177" spans="1:14">
       <c r="A177" t="s">
         <v>45</v>
       </c>
@@ -12364,7 +12370,7 @@
         <v>40329</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="15">
+    <row r="178" spans="1:14">
       <c r="A178" t="s">
         <v>553</v>
       </c>
@@ -12408,7 +12414,7 @@
         <v>40178</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="15">
+    <row r="179" spans="1:14">
       <c r="A179" t="s">
         <v>88</v>
       </c>
@@ -12452,7 +12458,7 @@
         <v>39994</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="15">
+    <row r="180" spans="1:14">
       <c r="A180" t="s">
         <v>45</v>
       </c>
@@ -12496,7 +12502,7 @@
         <v>39994</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="15">
+    <row r="181" spans="1:14">
       <c r="A181" t="s">
         <v>36</v>
       </c>
@@ -12540,7 +12546,7 @@
         <v>39994</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="15">
+    <row r="182" spans="1:14">
       <c r="A182" t="s">
         <v>562</v>
       </c>
@@ -12584,7 +12590,7 @@
         <v>39813</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="15">
+    <row r="183" spans="1:14">
       <c r="A183" t="s">
         <v>45</v>
       </c>
@@ -12628,7 +12634,7 @@
         <v>39813</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="15">
+    <row r="184" spans="1:14">
       <c r="A184" t="s">
         <v>230</v>
       </c>
@@ -12672,7 +12678,7 @@
         <v>39629</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="15">
+    <row r="185" spans="1:14">
       <c r="A185" t="s">
         <v>230</v>
       </c>
@@ -12716,7 +12722,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="15">
+    <row r="186" spans="1:14">
       <c r="A186" t="s">
         <v>70</v>
       </c>
@@ -12760,7 +12766,7 @@
         <v>40086</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="15">
+    <row r="187" spans="1:14">
       <c r="A187" t="s">
         <v>573</v>
       </c>
@@ -12804,7 +12810,7 @@
         <v>40086</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="15">
+    <row r="188" spans="1:14">
       <c r="A188" t="s">
         <v>141</v>
       </c>
@@ -12848,7 +12854,7 @@
         <v>39507</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="15">
+    <row r="189" spans="1:14">
       <c r="A189" t="s">
         <v>579</v>
       </c>
@@ -12892,7 +12898,7 @@
         <v>39691</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="15">
+    <row r="190" spans="1:14">
       <c r="A190" t="s">
         <v>377</v>
       </c>
@@ -12936,7 +12942,7 @@
         <v>39933</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="15">
+    <row r="191" spans="1:14">
       <c r="A191" t="s">
         <v>528</v>
       </c>
@@ -12980,7 +12986,7 @@
         <v>39903</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="15">
+    <row r="192" spans="1:14">
       <c r="A192" t="s">
         <v>587</v>
       </c>
@@ -13024,7 +13030,7 @@
         <v>39872</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="15">
+    <row r="193" spans="1:14">
       <c r="A193" t="s">
         <v>336</v>
       </c>
@@ -13068,7 +13074,7 @@
         <v>40633</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="15">
+    <row r="194" spans="1:14">
       <c r="A194" t="s">
         <v>88</v>
       </c>
@@ -13112,7 +13118,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="15">
+    <row r="195" spans="1:14">
       <c r="A195" t="s">
         <v>14</v>
       </c>
@@ -13156,7 +13162,7 @@
         <v>39964</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="15">
+    <row r="196" spans="1:14">
       <c r="A196" t="s">
         <v>598</v>
       </c>
@@ -13200,7 +13206,7 @@
         <v>40329</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="15">
+    <row r="197" spans="1:14">
       <c r="A197" t="s">
         <v>14</v>
       </c>
@@ -13244,7 +13250,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="15">
+    <row r="198" spans="1:14">
       <c r="A198" t="s">
         <v>450</v>
       </c>
@@ -13288,7 +13294,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="15">
+    <row r="199" spans="1:14">
       <c r="A199" t="s">
         <v>14</v>
       </c>
@@ -13332,7 +13338,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="15">
+    <row r="200" spans="1:14">
       <c r="A200" t="s">
         <v>387</v>
       </c>
@@ -13376,7 +13382,7 @@
         <v>40086</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="15">
+    <row r="201" spans="1:14">
       <c r="A201" t="s">
         <v>387</v>
       </c>
@@ -13420,7 +13426,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="15">
+    <row r="202" spans="1:14">
       <c r="A202" t="s">
         <v>230</v>
       </c>
@@ -13464,7 +13470,7 @@
         <v>40056</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="15">
+    <row r="203" spans="1:14">
       <c r="A203" t="s">
         <v>88</v>
       </c>
@@ -13508,7 +13514,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="15">
+    <row r="204" spans="1:14">
       <c r="A204" t="s">
         <v>426</v>
       </c>
@@ -13552,7 +13558,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="15">
+    <row r="205" spans="1:14">
       <c r="A205" t="s">
         <v>426</v>
       </c>
@@ -13596,7 +13602,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="15">
+    <row r="206" spans="1:14">
       <c r="A206" t="s">
         <v>36</v>
       </c>
@@ -13640,7 +13646,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="15">
+    <row r="207" spans="1:14">
       <c r="A207" t="s">
         <v>230</v>
       </c>
@@ -13684,7 +13690,7 @@
         <v>39994</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="15">
+    <row r="208" spans="1:14">
       <c r="A208" t="s">
         <v>45</v>
       </c>
@@ -13728,7 +13734,7 @@
         <v>40178</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="15">
+    <row r="209" spans="1:14">
       <c r="A209" t="s">
         <v>191</v>
       </c>
@@ -13772,7 +13778,7 @@
         <v>39933</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="15">
+    <row r="210" spans="1:14">
       <c r="A210" t="s">
         <v>70</v>
       </c>
@@ -13816,7 +13822,7 @@
         <v>40451</v>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="15">
+    <row r="211" spans="1:14">
       <c r="A211" t="s">
         <v>70</v>
       </c>
@@ -13860,7 +13866,7 @@
         <v>40633</v>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="15">
+    <row r="212" spans="1:14">
       <c r="A212" t="s">
         <v>629</v>
       </c>
@@ -13904,7 +13910,7 @@
         <v>40178</v>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="15">
+    <row r="213" spans="1:14">
       <c r="A213" t="s">
         <v>29</v>
       </c>
@@ -13948,7 +13954,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="15">
+    <row r="214" spans="1:14">
       <c r="A214" t="s">
         <v>636</v>
       </c>
@@ -13992,7 +13998,7 @@
         <v>40451</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="15">
+    <row r="215" spans="1:14">
       <c r="A215" t="s">
         <v>450</v>
       </c>
@@ -14036,7 +14042,7 @@
         <v>39903</v>
       </c>
     </row>
-    <row r="216" spans="1:14" ht="15">
+    <row r="216" spans="1:14">
       <c r="A216" t="s">
         <v>643</v>
       </c>
@@ -14080,7 +14086,7 @@
         <v>39903</v>
       </c>
     </row>
-    <row r="217" spans="1:14" ht="15">
+    <row r="217" spans="1:14">
       <c r="A217" t="s">
         <v>587</v>
       </c>
@@ -14124,7 +14130,7 @@
         <v>40237</v>
       </c>
     </row>
-    <row r="218" spans="1:14" ht="15">
+    <row r="218" spans="1:14">
       <c r="A218" t="s">
         <v>650</v>
       </c>
@@ -14168,7 +14174,7 @@
         <v>40209</v>
       </c>
     </row>
-    <row r="219" spans="1:14" ht="15">
+    <row r="219" spans="1:14">
       <c r="A219" t="s">
         <v>88</v>
       </c>
@@ -14212,7 +14218,7 @@
         <v>40724</v>
       </c>
     </row>
-    <row r="220" spans="1:14" ht="15">
+    <row r="220" spans="1:14">
       <c r="A220" t="s">
         <v>14</v>
       </c>
@@ -14256,7 +14262,7 @@
         <v>40329</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="15">
+    <row r="221" spans="1:14">
       <c r="A221" t="s">
         <v>450</v>
       </c>
@@ -14300,7 +14306,7 @@
         <v>40482</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="15">
+    <row r="222" spans="1:14">
       <c r="A222" t="s">
         <v>23</v>
       </c>
@@ -14344,7 +14350,7 @@
         <v>40908</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="15">
+    <row r="223" spans="1:14">
       <c r="A223" t="s">
         <v>598</v>
       </c>
@@ -14388,7 +14394,7 @@
         <v>40694</v>
       </c>
     </row>
-    <row r="224" spans="1:14" ht="15">
+    <row r="224" spans="1:14">
       <c r="A224" t="s">
         <v>14</v>
       </c>
@@ -14432,7 +14438,7 @@
         <v>40724</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="15">
+    <row r="225" spans="1:14">
       <c r="A225" t="s">
         <v>387</v>
       </c>
@@ -14476,7 +14482,7 @@
         <v>40451</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="15">
+    <row r="226" spans="1:14">
       <c r="A226" t="s">
         <v>36</v>
       </c>
@@ -14520,7 +14526,7 @@
         <v>41152</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="15">
+    <row r="227" spans="1:14">
       <c r="A227" t="s">
         <v>230</v>
       </c>
@@ -14564,7 +14570,7 @@
         <v>40329</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="15">
+    <row r="228" spans="1:14">
       <c r="A228" t="s">
         <v>159</v>
       </c>
@@ -14608,7 +14614,7 @@
         <v>40755</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="15">
+    <row r="229" spans="1:14">
       <c r="A229" t="s">
         <v>88</v>
       </c>
@@ -14652,7 +14658,7 @@
         <v>40724</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="15">
+    <row r="230" spans="1:14">
       <c r="A230" t="s">
         <v>677</v>
       </c>
@@ -14696,7 +14702,7 @@
         <v>40694</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="15">
+    <row r="231" spans="1:14">
       <c r="A231" t="s">
         <v>682</v>
       </c>
@@ -14740,7 +14746,7 @@
         <v>41090</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="15">
+    <row r="232" spans="1:14">
       <c r="A232" t="s">
         <v>687</v>
       </c>
@@ -14784,7 +14790,7 @@
         <v>40724</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="15">
+    <row r="233" spans="1:14">
       <c r="A233" t="s">
         <v>426</v>
       </c>
@@ -14828,7 +14834,7 @@
         <v>40724</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="15">
+    <row r="234" spans="1:14">
       <c r="A234" t="s">
         <v>36</v>
       </c>
@@ -14872,7 +14878,7 @@
         <v>40724</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="15">
+    <row r="235" spans="1:14">
       <c r="A235" t="s">
         <v>696</v>
       </c>
@@ -14916,7 +14922,7 @@
         <v>40543</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="15">
+    <row r="236" spans="1:14">
       <c r="A236" t="s">
         <v>230</v>
       </c>
@@ -14960,7 +14966,7 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="15">
+    <row r="237" spans="1:14">
       <c r="A237" t="s">
         <v>702</v>
       </c>
@@ -15004,7 +15010,7 @@
         <v>40543</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="15">
+    <row r="238" spans="1:14">
       <c r="A238" t="s">
         <v>191</v>
       </c>
@@ -15048,7 +15054,7 @@
         <v>40298</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="15">
+    <row r="239" spans="1:14">
       <c r="A239" t="s">
         <v>650</v>
       </c>
@@ -15092,7 +15098,7 @@
         <v>40663</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="15">
+    <row r="240" spans="1:14">
       <c r="A240" t="s">
         <v>587</v>
       </c>
@@ -15136,7 +15142,7 @@
         <v>40663</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="15">
+    <row r="241" spans="1:14">
       <c r="A241" t="s">
         <v>94</v>
       </c>
@@ -15180,7 +15186,7 @@
         <v>40694</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="15">
+    <row r="242" spans="1:14">
       <c r="A242" t="s">
         <v>70</v>
       </c>
@@ -15224,7 +15230,7 @@
         <v>40816</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="15">
+    <row r="243" spans="1:14">
       <c r="A243" t="s">
         <v>629</v>
       </c>
@@ -15268,7 +15274,7 @@
         <v>40543</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="15">
+    <row r="244" spans="1:14">
       <c r="A244" t="s">
         <v>719</v>
       </c>
@@ -15312,7 +15318,7 @@
         <v>40543</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="15">
+    <row r="245" spans="1:14">
       <c r="A245" t="s">
         <v>88</v>
       </c>
@@ -15356,7 +15362,7 @@
         <v>41090</v>
       </c>
     </row>
-    <row r="246" spans="1:14" ht="15">
+    <row r="246" spans="1:14">
       <c r="A246" t="s">
         <v>336</v>
       </c>
@@ -15400,7 +15406,7 @@
         <v>41486</v>
       </c>
     </row>
-    <row r="247" spans="1:14" ht="15">
+    <row r="247" spans="1:14">
       <c r="A247" t="s">
         <v>23</v>
       </c>
@@ -15444,7 +15450,7 @@
         <v>41090</v>
       </c>
     </row>
-    <row r="248" spans="1:14" ht="15">
+    <row r="248" spans="1:14">
       <c r="A248" t="s">
         <v>14</v>
       </c>
@@ -15488,7 +15494,7 @@
         <v>41090</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="15">
+    <row r="249" spans="1:14">
       <c r="A249" t="s">
         <v>731</v>
       </c>
@@ -15532,7 +15538,7 @@
         <v>41060</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="15">
+    <row r="250" spans="1:14">
       <c r="A250" t="s">
         <v>387</v>
       </c>
@@ -15576,7 +15582,7 @@
         <v>40847</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="15">
+    <row r="251" spans="1:14">
       <c r="A251" t="s">
         <v>29</v>
       </c>
@@ -15620,7 +15626,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="252" spans="1:14" ht="15">
+    <row r="252" spans="1:14">
       <c r="A252" t="s">
         <v>739</v>
       </c>
@@ -15664,7 +15670,7 @@
         <v>41213</v>
       </c>
     </row>
-    <row r="253" spans="1:14" ht="15">
+    <row r="253" spans="1:14">
       <c r="A253" t="s">
         <v>88</v>
       </c>
@@ -15708,7 +15714,7 @@
         <v>41090</v>
       </c>
     </row>
-    <row r="254" spans="1:14" ht="15">
+    <row r="254" spans="1:14">
       <c r="A254" t="s">
         <v>677</v>
       </c>
@@ -15752,7 +15758,7 @@
         <v>41090</v>
       </c>
     </row>
-    <row r="255" spans="1:14" ht="15">
+    <row r="255" spans="1:14">
       <c r="A255" t="s">
         <v>36</v>
       </c>
@@ -15796,7 +15802,7 @@
         <v>41090</v>
       </c>
     </row>
-    <row r="256" spans="1:14" ht="15">
+    <row r="256" spans="1:14">
       <c r="A256" t="s">
         <v>45</v>
       </c>
@@ -15840,7 +15846,7 @@
         <v>41029</v>
       </c>
     </row>
-    <row r="257" spans="1:14" ht="15">
+    <row r="257" spans="1:14">
       <c r="A257" t="s">
         <v>191</v>
       </c>
@@ -15884,7 +15890,7 @@
         <v>40663</v>
       </c>
     </row>
-    <row r="258" spans="1:14" ht="15">
+    <row r="258" spans="1:14">
       <c r="A258" t="s">
         <v>755</v>
       </c>
@@ -15928,7 +15934,7 @@
         <v>41333</v>
       </c>
     </row>
-    <row r="259" spans="1:14" ht="15">
+    <row r="259" spans="1:14">
       <c r="A259" t="s">
         <v>759</v>
       </c>
@@ -15972,7 +15978,7 @@
         <v>41274</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="15">
+    <row r="260" spans="1:14">
       <c r="A260" t="s">
         <v>255</v>
       </c>
@@ -16016,7 +16022,7 @@
         <v>41213</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="15">
+    <row r="261" spans="1:14">
       <c r="A261" t="s">
         <v>650</v>
       </c>
@@ -16060,7 +16066,7 @@
         <v>41060</v>
       </c>
     </row>
-    <row r="262" spans="1:14" ht="15">
+    <row r="262" spans="1:14">
       <c r="A262" t="s">
         <v>70</v>
       </c>
@@ -16104,7 +16110,7 @@
         <v>41182</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="15">
+    <row r="263" spans="1:14">
       <c r="A263" t="s">
         <v>629</v>
       </c>
@@ -16148,7 +16154,7 @@
         <v>40908</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="15">
+    <row r="264" spans="1:14">
       <c r="A264" t="s">
         <v>29</v>
       </c>
@@ -16192,7 +16198,7 @@
         <v>41274</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="15">
+    <row r="265" spans="1:14">
       <c r="A265" t="s">
         <v>771</v>
       </c>
@@ -16236,7 +16242,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="266" spans="1:14" ht="15">
+    <row r="266" spans="1:14">
       <c r="A266" t="s">
         <v>141</v>
       </c>
@@ -16280,7 +16286,7 @@
         <v>40755</v>
       </c>
     </row>
-    <row r="267" spans="1:14" ht="15">
+    <row r="267" spans="1:14">
       <c r="A267" t="s">
         <v>336</v>
       </c>
@@ -16324,7 +16330,7 @@
         <v>41943</v>
       </c>
     </row>
-    <row r="268" spans="1:14" ht="15">
+    <row r="268" spans="1:14">
       <c r="A268" t="s">
         <v>23</v>
       </c>
@@ -16368,7 +16374,7 @@
         <v>41274</v>
       </c>
     </row>
-    <row r="269" spans="1:14" ht="15">
+    <row r="269" spans="1:14">
       <c r="A269" t="s">
         <v>387</v>
       </c>
@@ -16412,7 +16418,7 @@
         <v>41213</v>
       </c>
     </row>
-    <row r="270" spans="1:14" ht="15">
+    <row r="270" spans="1:14">
       <c r="A270" t="s">
         <v>45</v>
       </c>
@@ -16456,7 +16462,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="271" spans="1:14" ht="15">
+    <row r="271" spans="1:14">
       <c r="A271" t="s">
         <v>739</v>
       </c>
@@ -16500,7 +16506,7 @@
         <v>41547</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="15">
+    <row r="272" spans="1:14">
       <c r="A272" t="s">
         <v>790</v>
       </c>
@@ -16544,7 +16550,7 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="273" spans="1:14" ht="15">
+    <row r="273" spans="1:14">
       <c r="A273" t="s">
         <v>159</v>
       </c>
@@ -16588,7 +16594,7 @@
         <v>41790</v>
       </c>
     </row>
-    <row r="274" spans="1:14" ht="15">
+    <row r="274" spans="1:14">
       <c r="A274" t="s">
         <v>88</v>
       </c>
@@ -16632,7 +16638,7 @@
         <v>41455</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="15">
+    <row r="275" spans="1:14">
       <c r="A275" t="s">
         <v>528</v>
       </c>
@@ -16676,7 +16682,7 @@
         <v>41425</v>
       </c>
     </row>
-    <row r="276" spans="1:14" ht="15">
+    <row r="276" spans="1:14">
       <c r="A276" t="s">
         <v>677</v>
       </c>
@@ -16720,7 +16726,7 @@
         <v>41425</v>
       </c>
     </row>
-    <row r="277" spans="1:14" ht="15">
+    <row r="277" spans="1:14">
       <c r="A277" t="s">
         <v>45</v>
       </c>
@@ -16764,7 +16770,7 @@
         <v>41364</v>
       </c>
     </row>
-    <row r="278" spans="1:14" ht="15">
+    <row r="278" spans="1:14">
       <c r="A278" t="s">
         <v>587</v>
       </c>
@@ -16808,7 +16814,7 @@
         <v>41274</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="15">
+    <row r="279" spans="1:14">
       <c r="A279" t="s">
         <v>806</v>
       </c>
@@ -16852,7 +16858,7 @@
         <v>41425</v>
       </c>
     </row>
-    <row r="280" spans="1:14" ht="15">
+    <row r="280" spans="1:14">
       <c r="A280" t="s">
         <v>806</v>
       </c>
@@ -16896,7 +16902,7 @@
         <v>41394</v>
       </c>
     </row>
-    <row r="281" spans="1:14" ht="15">
+    <row r="281" spans="1:14">
       <c r="A281" t="s">
         <v>255</v>
       </c>
@@ -16940,7 +16946,7 @@
         <v>41517</v>
       </c>
     </row>
-    <row r="282" spans="1:14" ht="15">
+    <row r="282" spans="1:14">
       <c r="A282" t="s">
         <v>70</v>
       </c>
@@ -16984,7 +16990,7 @@
         <v>41547</v>
       </c>
     </row>
-    <row r="283" spans="1:14" ht="15">
+    <row r="283" spans="1:14">
       <c r="A283" t="s">
         <v>790</v>
       </c>
@@ -17028,7 +17034,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="284" spans="1:14" ht="15">
+    <row r="284" spans="1:14">
       <c r="A284" t="s">
         <v>771</v>
       </c>
@@ -17072,7 +17078,7 @@
         <v>40968</v>
       </c>
     </row>
-    <row r="285" spans="1:14" ht="15">
+    <row r="285" spans="1:14">
       <c r="A285" t="s">
         <v>141</v>
       </c>
@@ -17116,7 +17122,7 @@
         <v>41121</v>
       </c>
     </row>
-    <row r="286" spans="1:14" ht="15">
+    <row r="286" spans="1:14">
       <c r="A286" t="s">
         <v>822</v>
       </c>
@@ -17160,7 +17166,7 @@
         <v>41305</v>
       </c>
     </row>
-    <row r="287" spans="1:14" ht="15">
+    <row r="287" spans="1:14">
       <c r="A287" t="s">
         <v>450</v>
       </c>
@@ -17204,7 +17210,7 @@
         <v>41060</v>
       </c>
     </row>
-    <row r="288" spans="1:14" ht="15">
+    <row r="288" spans="1:14">
       <c r="A288" t="s">
         <v>336</v>
       </c>
@@ -17248,7 +17254,7 @@
         <v>42155</v>
       </c>
     </row>
-    <row r="289" spans="1:14" ht="15">
+    <row r="289" spans="1:14">
       <c r="A289" t="s">
         <v>450</v>
       </c>
@@ -17292,7 +17298,7 @@
         <v>41729</v>
       </c>
     </row>
-    <row r="290" spans="1:14" ht="15">
+    <row r="290" spans="1:14">
       <c r="A290" t="s">
         <v>387</v>
       </c>
@@ -17336,7 +17342,7 @@
         <v>41547</v>
       </c>
     </row>
-    <row r="291" spans="1:14" ht="15">
+    <row r="291" spans="1:14">
       <c r="A291" t="s">
         <v>45</v>
       </c>
@@ -17380,7 +17386,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="292" spans="1:14" ht="15">
+    <row r="292" spans="1:14">
       <c r="A292" t="s">
         <v>309</v>
       </c>
@@ -17424,7 +17430,7 @@
         <v>41820</v>
       </c>
     </row>
-    <row r="293" spans="1:14" ht="15">
+    <row r="293" spans="1:14">
       <c r="A293" t="s">
         <v>840</v>
       </c>
@@ -17468,7 +17474,7 @@
         <v>41790</v>
       </c>
     </row>
-    <row r="294" spans="1:14" ht="15">
+    <row r="294" spans="1:14">
       <c r="A294" t="s">
         <v>88</v>
       </c>
@@ -17512,7 +17518,7 @@
         <v>41820</v>
       </c>
     </row>
-    <row r="295" spans="1:14" ht="15">
+    <row r="295" spans="1:14">
       <c r="A295" t="s">
         <v>687</v>
       </c>
@@ -17556,7 +17562,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="296" spans="1:14" ht="15">
+    <row r="296" spans="1:14">
       <c r="A296" t="s">
         <v>528</v>
       </c>
@@ -17600,7 +17606,7 @@
         <v>41790</v>
       </c>
     </row>
-    <row r="297" spans="1:14" ht="15">
+    <row r="297" spans="1:14">
       <c r="A297" t="s">
         <v>677</v>
       </c>
@@ -17644,7 +17650,7 @@
         <v>41790</v>
       </c>
     </row>
-    <row r="298" spans="1:14" ht="15">
+    <row r="298" spans="1:14">
       <c r="A298" t="s">
         <v>45</v>
       </c>
@@ -17688,7 +17694,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="299" spans="1:14" ht="15">
+    <row r="299" spans="1:14">
       <c r="A299" t="s">
         <v>854</v>
       </c>
@@ -17732,7 +17738,7 @@
         <v>41578</v>
       </c>
     </row>
-    <row r="300" spans="1:14" ht="15">
+    <row r="300" spans="1:14">
       <c r="A300" t="s">
         <v>230</v>
       </c>
@@ -17776,7 +17782,7 @@
         <v>41455</v>
       </c>
     </row>
-    <row r="301" spans="1:14" ht="15">
+    <row r="301" spans="1:14">
       <c r="A301" t="s">
         <v>45</v>
       </c>
@@ -17820,7 +17826,7 @@
         <v>41759</v>
       </c>
     </row>
-    <row r="302" spans="1:14" ht="15">
+    <row r="302" spans="1:14">
       <c r="A302" t="s">
         <v>319</v>
       </c>
@@ -17864,7 +17870,7 @@
         <v>41790</v>
       </c>
     </row>
-    <row r="303" spans="1:14" ht="15">
+    <row r="303" spans="1:14">
       <c r="A303" t="s">
         <v>806</v>
       </c>
@@ -17908,7 +17914,7 @@
         <v>41820</v>
       </c>
     </row>
-    <row r="304" spans="1:14" ht="15">
+    <row r="304" spans="1:14">
       <c r="A304" t="s">
         <v>806</v>
       </c>
@@ -17952,7 +17958,7 @@
         <v>41759</v>
       </c>
     </row>
-    <row r="305" spans="1:14" ht="15">
+    <row r="305" spans="1:14">
       <c r="A305" t="s">
         <v>868</v>
       </c>
@@ -17996,7 +18002,7 @@
         <v>41912</v>
       </c>
     </row>
-    <row r="306" spans="1:14" ht="15">
+    <row r="306" spans="1:14">
       <c r="A306" t="s">
         <v>872</v>
       </c>
@@ -18040,7 +18046,7 @@
         <v>41759</v>
       </c>
     </row>
-    <row r="307" spans="1:14" ht="15">
+    <row r="307" spans="1:14">
       <c r="A307" t="s">
         <v>878</v>
       </c>
@@ -18084,7 +18090,7 @@
         <v>41790</v>
       </c>
     </row>
-    <row r="308" spans="1:14" ht="15">
+    <row r="308" spans="1:14">
       <c r="A308" t="s">
         <v>70</v>
       </c>
@@ -18128,7 +18134,7 @@
         <v>41912</v>
       </c>
     </row>
-    <row r="309" spans="1:14" ht="15">
+    <row r="309" spans="1:14">
       <c r="A309" t="s">
         <v>29</v>
       </c>
@@ -18172,7 +18178,7 @@
         <v>42035</v>
       </c>
     </row>
-    <row r="310" spans="1:14" ht="15">
+    <row r="310" spans="1:14">
       <c r="A310" t="s">
         <v>886</v>
       </c>
@@ -18216,7 +18222,7 @@
         <v>41425</v>
       </c>
     </row>
-    <row r="311" spans="1:14" ht="15">
+    <row r="311" spans="1:14">
       <c r="A311" t="s">
         <v>336</v>
       </c>
@@ -18260,7 +18266,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="312" spans="1:14" ht="15">
+    <row r="312" spans="1:14">
       <c r="A312" t="s">
         <v>23</v>
       </c>
@@ -18304,7 +18310,7 @@
         <v>41820</v>
       </c>
     </row>
-    <row r="313" spans="1:14" ht="15">
+    <row r="313" spans="1:14">
       <c r="A313" t="s">
         <v>14</v>
       </c>
@@ -18348,7 +18354,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="314" spans="1:14" ht="15">
+    <row r="314" spans="1:14">
       <c r="A314" t="s">
         <v>387</v>
       </c>
@@ -18392,7 +18398,7 @@
         <v>41912</v>
       </c>
     </row>
-    <row r="315" spans="1:14" ht="15">
+    <row r="315" spans="1:14">
       <c r="A315" t="s">
         <v>587</v>
       </c>
@@ -18436,7 +18442,7 @@
         <v>42035</v>
       </c>
     </row>
-    <row r="316" spans="1:14" ht="15">
+    <row r="316" spans="1:14">
       <c r="A316" t="s">
         <v>36</v>
       </c>
@@ -18480,7 +18486,7 @@
         <v>42613</v>
       </c>
     </row>
-    <row r="317" spans="1:14" ht="15">
+    <row r="317" spans="1:14">
       <c r="A317" t="s">
         <v>300</v>
       </c>
@@ -18524,7 +18530,7 @@
         <v>41882</v>
       </c>
     </row>
-    <row r="318" spans="1:14" ht="15">
+    <row r="318" spans="1:14">
       <c r="A318" t="s">
         <v>159</v>
       </c>
@@ -18568,7 +18574,7 @@
         <v>42978</v>
       </c>
     </row>
-    <row r="319" spans="1:14" ht="15">
+    <row r="319" spans="1:14">
       <c r="A319" t="s">
         <v>739</v>
       </c>
@@ -18612,7 +18618,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="320" spans="1:14" ht="15">
+    <row r="320" spans="1:14">
       <c r="A320" t="s">
         <v>88</v>
       </c>
@@ -18656,7 +18662,7 @@
         <v>42185</v>
       </c>
     </row>
-    <row r="321" spans="1:14" ht="15">
+    <row r="321" spans="1:14">
       <c r="A321" t="s">
         <v>677</v>
       </c>
@@ -18700,7 +18706,7 @@
         <v>42155</v>
       </c>
     </row>
-    <row r="322" spans="1:14" ht="15">
+    <row r="322" spans="1:14">
       <c r="A322" t="s">
         <v>528</v>
       </c>
@@ -18744,7 +18750,7 @@
         <v>42185</v>
       </c>
     </row>
-    <row r="323" spans="1:14" ht="15">
+    <row r="323" spans="1:14">
       <c r="A323" t="s">
         <v>914</v>
       </c>
@@ -18788,7 +18794,7 @@
         <v>42185</v>
       </c>
     </row>
-    <row r="324" spans="1:14" ht="15">
+    <row r="324" spans="1:14">
       <c r="A324" t="s">
         <v>919</v>
       </c>
@@ -18832,7 +18838,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="325" spans="1:14" ht="15">
+    <row r="325" spans="1:14">
       <c r="A325" t="s">
         <v>36</v>
       </c>
@@ -18876,7 +18882,7 @@
         <v>42185</v>
       </c>
     </row>
-    <row r="326" spans="1:14" ht="15">
+    <row r="326" spans="1:14">
       <c r="A326" t="s">
         <v>230</v>
       </c>
@@ -18920,7 +18926,7 @@
         <v>41820</v>
       </c>
     </row>
-    <row r="327" spans="1:14" ht="15">
+    <row r="327" spans="1:14">
       <c r="A327" t="s">
         <v>45</v>
       </c>
@@ -18964,7 +18970,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="328" spans="1:14" ht="15">
+    <row r="328" spans="1:14">
       <c r="A328" t="s">
         <v>45</v>
       </c>
@@ -19008,7 +19014,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="329" spans="1:14" ht="15">
+    <row r="329" spans="1:14">
       <c r="A329" t="s">
         <v>806</v>
       </c>
@@ -19052,7 +19058,7 @@
         <v>42185</v>
       </c>
     </row>
-    <row r="330" spans="1:14" ht="15">
+    <row r="330" spans="1:14">
       <c r="A330" t="s">
         <v>739</v>
       </c>
@@ -19096,7 +19102,7 @@
         <v>42155</v>
       </c>
     </row>
-    <row r="331" spans="1:14" ht="15">
+    <row r="331" spans="1:14">
       <c r="A331" t="s">
         <v>806</v>
       </c>
@@ -19140,7 +19146,7 @@
         <v>42155</v>
       </c>
     </row>
-    <row r="332" spans="1:14" ht="15">
+    <row r="332" spans="1:14">
       <c r="A332" t="s">
         <v>878</v>
       </c>
@@ -19184,7 +19190,7 @@
         <v>42155</v>
       </c>
     </row>
-    <row r="333" spans="1:14" ht="15">
+    <row r="333" spans="1:14">
       <c r="A333" t="s">
         <v>275</v>
       </c>
@@ -19228,7 +19234,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="334" spans="1:14" ht="15">
+    <row r="334" spans="1:14">
       <c r="A334" t="s">
         <v>70</v>
       </c>
@@ -19272,7 +19278,7 @@
         <v>42277</v>
       </c>
     </row>
-    <row r="335" spans="1:14" ht="15">
+    <row r="335" spans="1:14">
       <c r="A335" t="s">
         <v>790</v>
       </c>
@@ -19316,7 +19322,7 @@
         <v>42308</v>
       </c>
     </row>
-    <row r="336" spans="1:14" ht="15">
+    <row r="336" spans="1:14">
       <c r="A336" t="s">
         <v>309</v>
       </c>
@@ -19360,7 +19366,7 @@
         <v>41851</v>
       </c>
     </row>
-    <row r="337" spans="1:14" ht="15">
+    <row r="337" spans="1:14">
       <c r="A337" t="s">
         <v>450</v>
       </c>
@@ -19404,7 +19410,7 @@
         <v>41790</v>
       </c>
     </row>
-    <row r="338" spans="1:14" ht="15">
+    <row r="338" spans="1:14">
       <c r="A338" t="s">
         <v>643</v>
       </c>
@@ -19448,7 +19454,7 @@
         <v>42886</v>
       </c>
     </row>
-    <row r="339" spans="1:14" ht="15">
+    <row r="339" spans="1:14">
       <c r="A339" t="s">
         <v>23</v>
       </c>
@@ -19492,7 +19498,7 @@
         <v>42185</v>
       </c>
     </row>
-    <row r="340" spans="1:14" ht="15">
+    <row r="340" spans="1:14">
       <c r="A340" t="s">
         <v>14</v>
       </c>
@@ -19536,7 +19542,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="341" spans="1:14" ht="15">
+    <row r="341" spans="1:14">
       <c r="A341" t="s">
         <v>450</v>
       </c>
@@ -19580,7 +19586,7 @@
         <v>42277</v>
       </c>
     </row>
-    <row r="342" spans="1:14" ht="15">
+    <row r="342" spans="1:14">
       <c r="A342" t="s">
         <v>587</v>
       </c>
@@ -19624,7 +19630,7 @@
         <v>42400</v>
       </c>
     </row>
-    <row r="343" spans="1:14" ht="15">
+    <row r="343" spans="1:14">
       <c r="A343" t="s">
         <v>387</v>
       </c>
@@ -19668,7 +19674,7 @@
         <v>42308</v>
       </c>
     </row>
-    <row r="344" spans="1:14" ht="15">
+    <row r="344" spans="1:14">
       <c r="A344" t="s">
         <v>113</v>
       </c>
@@ -19712,7 +19718,7 @@
         <v>42185</v>
       </c>
     </row>
-    <row r="345" spans="1:14" ht="15">
+    <row r="345" spans="1:14">
       <c r="A345" t="s">
         <v>45</v>
       </c>
@@ -19756,7 +19762,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="346" spans="1:14" ht="15">
+    <row r="346" spans="1:14">
       <c r="A346" t="s">
         <v>966</v>
       </c>
@@ -19800,7 +19806,7 @@
         <v>42429</v>
       </c>
     </row>
-    <row r="347" spans="1:14" ht="15">
+    <row r="347" spans="1:14">
       <c r="A347" t="s">
         <v>88</v>
       </c>
@@ -19844,7 +19850,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="348" spans="1:14" ht="15">
+    <row r="348" spans="1:14">
       <c r="A348" t="s">
         <v>677</v>
       </c>
@@ -19888,7 +19894,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="349" spans="1:14" ht="15">
+    <row r="349" spans="1:14">
       <c r="A349" t="s">
         <v>528</v>
       </c>
@@ -19932,7 +19938,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="350" spans="1:14" ht="15">
+    <row r="350" spans="1:14">
       <c r="A350" t="s">
         <v>919</v>
       </c>
@@ -19976,7 +19982,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="351" spans="1:14" ht="15">
+    <row r="351" spans="1:14">
       <c r="A351" t="s">
         <v>36</v>
       </c>
@@ -20020,7 +20026,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="352" spans="1:14" ht="15">
+    <row r="352" spans="1:14">
       <c r="A352" t="s">
         <v>980</v>
       </c>
@@ -20064,7 +20070,7 @@
         <v>42460</v>
       </c>
     </row>
-    <row r="353" spans="1:14" ht="15">
+    <row r="353" spans="1:14">
       <c r="A353" t="s">
         <v>985</v>
       </c>
@@ -20108,7 +20114,7 @@
         <v>42247</v>
       </c>
     </row>
-    <row r="354" spans="1:14" ht="15">
+    <row r="354" spans="1:14">
       <c r="A354" t="s">
         <v>989</v>
       </c>
@@ -20152,7 +20158,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="355" spans="1:14" ht="15">
+    <row r="355" spans="1:14">
       <c r="A355" t="s">
         <v>45</v>
       </c>
@@ -20196,7 +20202,7 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="356" spans="1:14" ht="15">
+    <row r="356" spans="1:14">
       <c r="A356" t="s">
         <v>418</v>
       </c>
@@ -20240,7 +20246,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="357" spans="1:14" ht="15">
+    <row r="357" spans="1:14">
       <c r="A357" t="s">
         <v>806</v>
       </c>
@@ -20284,7 +20290,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="358" spans="1:14" ht="15">
+    <row r="358" spans="1:14">
       <c r="A358" t="s">
         <v>806</v>
       </c>
@@ -20328,7 +20334,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="359" spans="1:14" ht="15">
+    <row r="359" spans="1:14">
       <c r="A359" t="s">
         <v>878</v>
       </c>
@@ -20372,7 +20378,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="360" spans="1:14" ht="15">
+    <row r="360" spans="1:14">
       <c r="A360" t="s">
         <v>70</v>
       </c>
@@ -20416,7 +20422,7 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="361" spans="1:14" ht="15">
+    <row r="361" spans="1:14">
       <c r="A361" t="s">
         <v>29</v>
       </c>
@@ -20460,7 +20466,7 @@
         <v>42674</v>
       </c>
     </row>
-    <row r="362" spans="1:14" ht="15">
+    <row r="362" spans="1:14">
       <c r="A362" t="s">
         <v>230</v>
       </c>
@@ -20504,7 +20510,7 @@
         <v>42185</v>
       </c>
     </row>
-    <row r="363" spans="1:14" ht="15">
+    <row r="363" spans="1:14">
       <c r="A363" t="s">
         <v>790</v>
       </c>
@@ -20548,7 +20554,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="364" spans="1:14" ht="15">
+    <row r="364" spans="1:14">
       <c r="A364" t="s">
         <v>159</v>
       </c>
@@ -20592,7 +20598,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="365" spans="1:14" ht="15">
+    <row r="365" spans="1:14">
       <c r="A365" t="s">
         <v>1013</v>
       </c>
@@ -20636,7 +20642,7 @@
         <v>42063</v>
       </c>
     </row>
-    <row r="366" spans="1:14" ht="15">
+    <row r="366" spans="1:14">
       <c r="A366" t="s">
         <v>309</v>
       </c>
@@ -20680,7 +20686,7 @@
         <v>42247</v>
       </c>
     </row>
-    <row r="367" spans="1:14" ht="15">
+    <row r="367" spans="1:14">
       <c r="A367" t="s">
         <v>141</v>
       </c>
@@ -20724,7 +20730,7 @@
         <v>42216</v>
       </c>
     </row>
-    <row r="368" spans="1:14" ht="15">
+    <row r="368" spans="1:14">
       <c r="A368" t="s">
         <v>1022</v>
       </c>
@@ -20768,7 +20774,7 @@
         <v>42886</v>
       </c>
     </row>
-    <row r="369" spans="1:14" ht="15">
+    <row r="369" spans="1:14">
       <c r="A369" t="s">
         <v>336</v>
       </c>
@@ -20812,7 +20818,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="370" spans="1:14" ht="15">
+    <row r="370" spans="1:14">
       <c r="A370" t="s">
         <v>23</v>
       </c>
@@ -20856,7 +20862,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="371" spans="1:14" ht="15">
+    <row r="371" spans="1:14">
       <c r="A371" t="s">
         <v>14</v>
       </c>
@@ -20900,7 +20906,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="372" spans="1:14" ht="15">
+    <row r="372" spans="1:14">
       <c r="A372" t="s">
         <v>587</v>
       </c>
@@ -20944,7 +20950,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="373" spans="1:14" ht="15">
+    <row r="373" spans="1:14">
       <c r="A373" t="s">
         <v>387</v>
       </c>
@@ -20988,7 +20994,7 @@
         <v>42674</v>
       </c>
     </row>
-    <row r="374" spans="1:14" ht="15">
+    <row r="374" spans="1:14">
       <c r="A374" t="s">
         <v>113</v>
       </c>
@@ -21032,7 +21038,7 @@
         <v>42825</v>
       </c>
     </row>
-    <row r="375" spans="1:14" ht="15">
+    <row r="375" spans="1:14">
       <c r="A375" t="s">
         <v>45</v>
       </c>
@@ -21076,7 +21082,7 @@
         <v>43220</v>
       </c>
     </row>
-    <row r="376" spans="1:14" ht="15">
+    <row r="376" spans="1:14">
       <c r="A376" t="s">
         <v>45</v>
       </c>
@@ -21120,7 +21126,7 @@
         <v>42886</v>
       </c>
     </row>
-    <row r="377" spans="1:14" ht="15">
+    <row r="377" spans="1:14">
       <c r="A377" t="s">
         <v>300</v>
       </c>
@@ -21164,7 +21170,7 @@
         <v>43008</v>
       </c>
     </row>
-    <row r="378" spans="1:14" ht="15">
+    <row r="378" spans="1:14">
       <c r="A378" t="s">
         <v>528</v>
       </c>
@@ -21208,7 +21214,7 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="379" spans="1:14" ht="15">
+    <row r="379" spans="1:14">
       <c r="A379" t="s">
         <v>29</v>
       </c>
@@ -21252,7 +21258,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="380" spans="1:14" ht="15">
+    <row r="380" spans="1:14">
       <c r="A380" t="s">
         <v>1049</v>
       </c>
@@ -21296,7 +21302,7 @@
         <v>43312</v>
       </c>
     </row>
-    <row r="381" spans="1:14" ht="15">
+    <row r="381" spans="1:14">
       <c r="A381" t="s">
         <v>45</v>
       </c>
@@ -21340,7 +21346,7 @@
         <v>43220</v>
       </c>
     </row>
-    <row r="382" spans="1:14" ht="15">
+    <row r="382" spans="1:14">
       <c r="A382" t="s">
         <v>88</v>
       </c>
@@ -21384,7 +21390,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="383" spans="1:14" ht="15">
+    <row r="383" spans="1:14">
       <c r="A383" t="s">
         <v>528</v>
       </c>
@@ -21428,7 +21434,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="384" spans="1:14" ht="15">
+    <row r="384" spans="1:14">
       <c r="A384" t="s">
         <v>1059</v>
       </c>
@@ -21472,7 +21478,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="385" spans="1:14" ht="15">
+    <row r="385" spans="1:14">
       <c r="A385" t="s">
         <v>919</v>
       </c>
@@ -21516,7 +21522,7 @@
         <v>43190</v>
       </c>
     </row>
-    <row r="386" spans="1:14" ht="15">
+    <row r="386" spans="1:14">
       <c r="A386" t="s">
         <v>980</v>
       </c>
@@ -21560,7 +21566,7 @@
         <v>42825</v>
       </c>
     </row>
-    <row r="387" spans="1:14" ht="15">
+    <row r="387" spans="1:14">
       <c r="A387" t="s">
         <v>36</v>
       </c>
@@ -21604,7 +21610,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="388" spans="1:14" ht="15">
+    <row r="388" spans="1:14">
       <c r="A388" t="s">
         <v>1070</v>
       </c>
@@ -21648,7 +21654,7 @@
         <v>42704</v>
       </c>
     </row>
-    <row r="389" spans="1:14" ht="15">
+    <row r="389" spans="1:14">
       <c r="A389" t="s">
         <v>450</v>
       </c>
@@ -21692,7 +21698,7 @@
         <v>42794</v>
       </c>
     </row>
-    <row r="390" spans="1:14" ht="15">
+    <row r="390" spans="1:14">
       <c r="A390" t="s">
         <v>45</v>
       </c>
@@ -21736,7 +21742,7 @@
         <v>42886</v>
       </c>
     </row>
-    <row r="391" spans="1:14" ht="15">
+    <row r="391" spans="1:14">
       <c r="A391" t="s">
         <v>1078</v>
       </c>
@@ -21780,7 +21786,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="392" spans="1:14" ht="15">
+    <row r="392" spans="1:14">
       <c r="A392" t="s">
         <v>1082</v>
       </c>
@@ -21824,7 +21830,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="393" spans="1:14" ht="15">
+    <row r="393" spans="1:14">
       <c r="A393" t="s">
         <v>418</v>
       </c>
@@ -21868,7 +21874,7 @@
         <v>42886</v>
       </c>
     </row>
-    <row r="394" spans="1:14" ht="15">
+    <row r="394" spans="1:14">
       <c r="A394" t="s">
         <v>806</v>
       </c>
@@ -21912,7 +21918,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="395" spans="1:14" ht="15">
+    <row r="395" spans="1:14">
       <c r="A395" t="s">
         <v>1090</v>
       </c>
@@ -21956,7 +21962,7 @@
         <v>42855</v>
       </c>
     </row>
-    <row r="396" spans="1:14" ht="15">
+    <row r="396" spans="1:14">
       <c r="A396" t="s">
         <v>70</v>
       </c>
@@ -22000,7 +22006,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="397" spans="1:14" ht="15">
+    <row r="397" spans="1:14">
       <c r="A397" t="s">
         <v>230</v>
       </c>
@@ -22044,7 +22050,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="398" spans="1:14" ht="15">
+    <row r="398" spans="1:14">
       <c r="A398" t="s">
         <v>29</v>
       </c>
@@ -22088,7 +22094,7 @@
         <v>43069</v>
       </c>
     </row>
-    <row r="399" spans="1:14" ht="15">
+    <row r="399" spans="1:14">
       <c r="A399" t="s">
         <v>790</v>
       </c>
@@ -22132,7 +22138,7 @@
         <v>43039</v>
       </c>
     </row>
-    <row r="400" spans="1:14" ht="15">
+    <row r="400" spans="1:14">
       <c r="A400" t="s">
         <v>159</v>
       </c>
@@ -22176,7 +22182,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="401" spans="1:14" ht="15">
+    <row r="401" spans="1:14">
       <c r="A401" t="s">
         <v>579</v>
       </c>
@@ -22220,7 +22226,7 @@
         <v>42490</v>
       </c>
     </row>
-    <row r="402" spans="1:14" ht="15">
+    <row r="402" spans="1:14">
       <c r="A402" t="s">
         <v>141</v>
       </c>
@@ -22264,7 +22270,7 @@
         <v>42674</v>
       </c>
     </row>
-    <row r="403" spans="1:14" ht="15">
+    <row r="403" spans="1:14">
       <c r="A403" t="s">
         <v>1107</v>
       </c>
@@ -22308,7 +22314,7 @@
         <v>42400</v>
       </c>
     </row>
-    <row r="404" spans="1:14" ht="15">
+    <row r="404" spans="1:14">
       <c r="A404" t="s">
         <v>336</v>
       </c>
@@ -22352,7 +22358,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="405" spans="1:14" ht="15">
+    <row r="405" spans="1:14">
       <c r="A405" t="s">
         <v>643</v>
       </c>
@@ -22396,7 +22402,7 @@
         <v>43616</v>
       </c>
     </row>
-    <row r="406" spans="1:14" ht="15">
+    <row r="406" spans="1:14">
       <c r="A406" t="s">
         <v>23</v>
       </c>
@@ -22440,7 +22446,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="407" spans="1:14" ht="15">
+    <row r="407" spans="1:14">
       <c r="A407" t="s">
         <v>387</v>
       </c>
@@ -22484,7 +22490,7 @@
         <v>43039</v>
       </c>
     </row>
-    <row r="408" spans="1:14" ht="15">
+    <row r="408" spans="1:14">
       <c r="A408" t="s">
         <v>587</v>
       </c>
@@ -22528,7 +22534,7 @@
         <v>43131</v>
       </c>
     </row>
-    <row r="409" spans="1:14" ht="15">
+    <row r="409" spans="1:14">
       <c r="A409" t="s">
         <v>1122</v>
       </c>
@@ -22572,7 +22578,7 @@
         <v>42855</v>
       </c>
     </row>
-    <row r="410" spans="1:14" ht="15">
+    <row r="410" spans="1:14">
       <c r="A410" t="s">
         <v>1126</v>
       </c>
@@ -22616,7 +22622,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="411" spans="1:14" ht="15">
+    <row r="411" spans="1:14">
       <c r="A411" t="s">
         <v>739</v>
       </c>
@@ -22660,7 +22666,7 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="412" spans="1:14" ht="15">
+    <row r="412" spans="1:14">
       <c r="A412" t="s">
         <v>45</v>
       </c>
@@ -22704,7 +22710,7 @@
         <v>44135</v>
       </c>
     </row>
-    <row r="413" spans="1:14" ht="15">
+    <row r="413" spans="1:14">
       <c r="A413" t="s">
         <v>305</v>
       </c>
@@ -22748,7 +22754,7 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="414" spans="1:14" ht="15">
+    <row r="414" spans="1:14">
       <c r="A414" t="s">
         <v>88</v>
       </c>
@@ -22792,7 +22798,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="415" spans="1:14" ht="15">
+    <row r="415" spans="1:14">
       <c r="A415" t="s">
         <v>919</v>
       </c>
@@ -22836,7 +22842,7 @@
         <v>43190</v>
       </c>
     </row>
-    <row r="416" spans="1:14" ht="15">
+    <row r="416" spans="1:14">
       <c r="A416" t="s">
         <v>36</v>
       </c>
@@ -22880,7 +22886,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="417" spans="1:14" ht="15">
+    <row r="417" spans="1:14">
       <c r="A417" t="s">
         <v>1143</v>
       </c>
@@ -22924,7 +22930,7 @@
         <v>43039</v>
       </c>
     </row>
-    <row r="418" spans="1:14" ht="15">
+    <row r="418" spans="1:14">
       <c r="A418" t="s">
         <v>36</v>
       </c>
@@ -22968,7 +22974,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="419" spans="1:14" ht="15">
+    <row r="419" spans="1:14">
       <c r="A419" t="s">
         <v>1149</v>
       </c>
@@ -23012,7 +23018,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="420" spans="1:14" ht="15">
+    <row r="420" spans="1:14">
       <c r="A420" t="s">
         <v>989</v>
       </c>
@@ -23056,7 +23062,7 @@
         <v>43343</v>
       </c>
     </row>
-    <row r="421" spans="1:14" ht="15">
+    <row r="421" spans="1:14">
       <c r="A421" t="s">
         <v>36</v>
       </c>
@@ -23100,7 +23106,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="422" spans="1:14" ht="15">
+    <row r="422" spans="1:14">
       <c r="A422" t="s">
         <v>418</v>
       </c>
@@ -23144,7 +23150,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="423" spans="1:14" ht="15">
+    <row r="423" spans="1:14">
       <c r="A423" t="s">
         <v>806</v>
       </c>
@@ -23188,7 +23194,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="424" spans="1:14" ht="15">
+    <row r="424" spans="1:14">
       <c r="A424" t="s">
         <v>806</v>
       </c>
@@ -23232,7 +23238,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="425" spans="1:14" ht="15">
+    <row r="425" spans="1:14">
       <c r="A425" t="s">
         <v>1090</v>
       </c>
@@ -23276,7 +23282,7 @@
         <v>43190</v>
       </c>
     </row>
-    <row r="426" spans="1:14" ht="15">
+    <row r="426" spans="1:14">
       <c r="A426" t="s">
         <v>70</v>
       </c>
@@ -23320,7 +23326,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="427" spans="1:14" ht="15">
+    <row r="427" spans="1:14">
       <c r="A427" t="s">
         <v>230</v>
       </c>
@@ -23364,7 +23370,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="428" spans="1:14" ht="15">
+    <row r="428" spans="1:14">
       <c r="A428" t="s">
         <v>141</v>
       </c>
@@ -23408,7 +23414,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="429" spans="1:14" ht="15">
+    <row r="429" spans="1:14">
       <c r="A429" t="s">
         <v>159</v>
       </c>
@@ -23452,7 +23458,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="430" spans="1:14" ht="15">
+    <row r="430" spans="1:14">
       <c r="A430" t="s">
         <v>1173</v>
       </c>
@@ -23496,7 +23502,7 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="431" spans="1:14" ht="15">
+    <row r="431" spans="1:14">
       <c r="A431" t="s">
         <v>1013</v>
       </c>
@@ -23540,7 +23546,7 @@
         <v>42825</v>
       </c>
     </row>
-    <row r="432" spans="1:14" ht="15">
+    <row r="432" spans="1:14">
       <c r="A432" t="s">
         <v>966</v>
       </c>
@@ -23584,7 +23590,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="433" spans="1:14" ht="15">
+    <row r="433" spans="1:14">
       <c r="A433" t="s">
         <v>1181</v>
       </c>
@@ -23628,7 +23634,7 @@
         <v>42916</v>
       </c>
     </row>
-    <row r="434" spans="1:14" ht="15">
+    <row r="434" spans="1:14">
       <c r="A434" t="s">
         <v>450</v>
       </c>
@@ -23672,7 +23678,7 @@
         <v>42886</v>
       </c>
     </row>
-    <row r="435" spans="1:14" ht="15">
+    <row r="435" spans="1:14">
       <c r="A435" t="s">
         <v>1059</v>
       </c>
@@ -23716,7 +23722,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="436" spans="1:14" ht="15">
+    <row r="436" spans="1:14">
       <c r="A436" t="s">
         <v>387</v>
       </c>
@@ -23760,7 +23766,7 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="437" spans="1:14" ht="15">
+    <row r="437" spans="1:14">
       <c r="A437" t="s">
         <v>113</v>
       </c>
@@ -23804,7 +23810,7 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="438" spans="1:14" ht="15">
+    <row r="438" spans="1:14">
       <c r="A438" t="s">
         <v>36</v>
       </c>
@@ -23848,7 +23854,7 @@
         <v>44012</v>
       </c>
     </row>
-    <row r="439" spans="1:14" ht="15">
+    <row r="439" spans="1:14">
       <c r="A439" t="s">
         <v>806</v>
       </c>
@@ -23892,7 +23898,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="440" spans="1:14" ht="15">
+    <row r="440" spans="1:14">
       <c r="A440" t="s">
         <v>336</v>
       </c>
@@ -23936,7 +23942,7 @@
         <v>44012</v>
       </c>
     </row>
-    <row r="441" spans="1:14" ht="15">
+    <row r="441" spans="1:14">
       <c r="A441" t="s">
         <v>159</v>
       </c>
@@ -23980,7 +23986,7 @@
         <v>44196</v>
       </c>
     </row>
-    <row r="442" spans="1:14" ht="15">
+    <row r="442" spans="1:14">
       <c r="A442" t="s">
         <v>980</v>
       </c>
@@ -24024,7 +24030,7 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="443" spans="1:14" ht="15">
+    <row r="443" spans="1:14">
       <c r="A443" t="s">
         <v>159</v>
       </c>
@@ -24068,7 +24074,7 @@
         <v>44043</v>
       </c>
     </row>
-    <row r="444" spans="1:14" ht="15">
+    <row r="444" spans="1:14">
       <c r="A444" t="s">
         <v>528</v>
       </c>
@@ -24112,7 +24118,7 @@
         <v>43738</v>
       </c>
     </row>
-    <row r="445" spans="1:14" ht="15">
+    <row r="445" spans="1:14">
       <c r="A445" t="s">
         <v>806</v>
       </c>
@@ -24156,7 +24162,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="446" spans="1:14" ht="15">
+    <row r="446" spans="1:14">
       <c r="A446" t="s">
         <v>70</v>
       </c>
@@ -24200,7 +24206,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="447" spans="1:14" ht="15">
+    <row r="447" spans="1:14">
       <c r="A447" t="s">
         <v>1215</v>
       </c>
@@ -24244,7 +24250,7 @@
         <v>43434</v>
       </c>
     </row>
-    <row r="448" spans="1:14" ht="15">
+    <row r="448" spans="1:14">
       <c r="A448" t="s">
         <v>1219</v>
       </c>
@@ -24288,7 +24294,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="449" spans="1:14" ht="15">
+    <row r="449" spans="1:14">
       <c r="A449" t="s">
         <v>1223</v>
       </c>
@@ -24332,7 +24338,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="450" spans="1:14" ht="15">
+    <row r="450" spans="1:14">
       <c r="A450" t="s">
         <v>1226</v>
       </c>
@@ -24376,7 +24382,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="451" spans="1:14" ht="15">
+    <row r="451" spans="1:14">
       <c r="A451" t="s">
         <v>88</v>
       </c>
@@ -24420,7 +24426,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="452" spans="1:14" ht="15">
+    <row r="452" spans="1:14">
       <c r="A452" t="s">
         <v>1070</v>
       </c>
@@ -24464,7 +24470,7 @@
         <v>43434</v>
       </c>
     </row>
-    <row r="453" spans="1:14" ht="15">
+    <row r="453" spans="1:14">
       <c r="A453" t="s">
         <v>23</v>
       </c>
@@ -24508,7 +24514,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="454" spans="1:14" ht="15">
+    <row r="454" spans="1:14">
       <c r="A454" t="s">
         <v>1126</v>
       </c>
@@ -24552,7 +24558,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="455" spans="1:14" ht="15">
+    <row r="455" spans="1:14">
       <c r="A455" t="s">
         <v>450</v>
       </c>
@@ -24596,7 +24602,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="456" spans="1:14" ht="15">
+    <row r="456" spans="1:14">
       <c r="A456" t="s">
         <v>1107</v>
       </c>
@@ -24640,7 +24646,7 @@
         <v>43434</v>
       </c>
     </row>
-    <row r="457" spans="1:14" ht="15">
+    <row r="457" spans="1:14">
       <c r="A457" t="s">
         <v>141</v>
       </c>
@@ -24684,7 +24690,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="458" spans="1:14" ht="15">
+    <row r="458" spans="1:14">
       <c r="A458" t="s">
         <v>579</v>
       </c>
@@ -24728,7 +24734,7 @@
         <v>43131</v>
       </c>
     </row>
-    <row r="459" spans="1:14" ht="15">
+    <row r="459" spans="1:14">
       <c r="A459" t="s">
         <v>1013</v>
       </c>
@@ -24772,7 +24778,7 @@
         <v>43190</v>
       </c>
     </row>
-    <row r="460" spans="1:14" ht="15">
+    <row r="460" spans="1:14">
       <c r="A460" t="s">
         <v>1126</v>
       </c>
@@ -24816,7 +24822,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="461" spans="1:14" ht="15">
+    <row r="461" spans="1:14">
       <c r="A461" t="s">
         <v>36</v>
       </c>
@@ -24860,7 +24866,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="462" spans="1:14" ht="15">
+    <row r="462" spans="1:14">
       <c r="A462" t="s">
         <v>23</v>
       </c>
@@ -24904,7 +24910,7 @@
         <v>44196</v>
       </c>
     </row>
-    <row r="463" spans="1:14" ht="15">
+    <row r="463" spans="1:14">
       <c r="A463" t="s">
         <v>790</v>
       </c>
@@ -24948,7 +24954,7 @@
         <v>44165</v>
       </c>
     </row>
-    <row r="464" spans="1:14" ht="15">
+    <row r="464" spans="1:14">
       <c r="A464" t="s">
         <v>305</v>
       </c>
@@ -24992,7 +24998,7 @@
         <v>44074</v>
       </c>
     </row>
-    <row r="465" spans="1:14" ht="15">
+    <row r="465" spans="1:14">
       <c r="A465" t="s">
         <v>450</v>
       </c>
@@ -25036,7 +25042,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="466" spans="1:14" ht="15">
+    <row r="466" spans="1:14">
       <c r="A466" t="s">
         <v>840</v>
       </c>
@@ -25080,7 +25086,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="467" spans="1:14" ht="15">
+    <row r="467" spans="1:14">
       <c r="A467" t="s">
         <v>1090</v>
       </c>
@@ -25124,7 +25130,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="468" spans="1:14" ht="15">
+    <row r="468" spans="1:14">
       <c r="A468" t="s">
         <v>1013</v>
       </c>
@@ -25168,7 +25174,7 @@
         <v>43616</v>
       </c>
     </row>
-    <row r="469" spans="1:14" ht="15">
+    <row r="469" spans="1:14">
       <c r="A469" t="s">
         <v>1268</v>
       </c>
@@ -25212,7 +25218,7 @@
         <v>43738</v>
       </c>
     </row>
-    <row r="470" spans="1:14" ht="15">
+    <row r="470" spans="1:14">
       <c r="A470" t="s">
         <v>1059</v>
       </c>
@@ -25256,7 +25262,7 @@
         <v>44012</v>
       </c>
     </row>
-    <row r="471" spans="1:14" ht="15">
+    <row r="471" spans="1:14">
       <c r="A471" t="s">
         <v>141</v>
       </c>
@@ -25300,7 +25306,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="472" spans="1:14" ht="15">
+    <row r="472" spans="1:14">
       <c r="A472" t="s">
         <v>387</v>
       </c>
@@ -25344,7 +25350,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="473" spans="1:14" ht="15">
+    <row r="473" spans="1:14">
       <c r="A473" t="s">
         <v>537</v>
       </c>
@@ -25388,7 +25394,7 @@
         <v>43982</v>
       </c>
     </row>
-    <row r="474" spans="1:14" ht="15">
+    <row r="474" spans="1:14">
       <c r="A474" t="s">
         <v>1281</v>
       </c>
@@ -25432,7 +25438,7 @@
         <v>44196</v>
       </c>
     </row>
-    <row r="475" spans="1:14" ht="15">
+    <row r="475" spans="1:14">
       <c r="A475" t="s">
         <v>587</v>
       </c>
@@ -25476,7 +25482,7 @@
         <v>43982</v>
       </c>
     </row>
-    <row r="476" spans="1:14" ht="15">
+    <row r="476" spans="1:14">
       <c r="A476" t="s">
         <v>528</v>
       </c>
@@ -25520,7 +25526,7 @@
         <v>44012</v>
       </c>
     </row>
-    <row r="477" spans="1:14" ht="15">
+    <row r="477" spans="1:14">
       <c r="A477" t="s">
         <v>980</v>
       </c>
@@ -25564,7 +25570,7 @@
         <v>43921</v>
       </c>
     </row>
-    <row r="478" spans="1:14" ht="15">
+    <row r="478" spans="1:14">
       <c r="A478" t="s">
         <v>1291</v>
       </c>
@@ -25608,7 +25614,7 @@
         <v>43951</v>
       </c>
     </row>
-    <row r="479" spans="1:14" ht="15">
+    <row r="479" spans="1:14">
       <c r="A479" t="s">
         <v>806</v>
       </c>
@@ -25652,7 +25658,7 @@
         <v>44012</v>
       </c>
     </row>
-    <row r="480" spans="1:14" ht="15">
+    <row r="480" spans="1:14">
       <c r="A480" t="s">
         <v>230</v>
       </c>
@@ -25696,7 +25702,7 @@
         <v>43890</v>
       </c>
     </row>
-    <row r="481" spans="1:14" ht="15">
+    <row r="481" spans="1:14">
       <c r="A481" t="s">
         <v>159</v>
       </c>
@@ -25740,7 +25746,7 @@
         <v>44377</v>
       </c>
     </row>
-    <row r="482" spans="1:14" ht="15">
+    <row r="482" spans="1:14">
       <c r="A482" t="s">
         <v>159</v>
       </c>
@@ -25784,7 +25790,7 @@
         <v>44408</v>
       </c>
     </row>
-    <row r="483" spans="1:14" ht="15">
+    <row r="483" spans="1:14">
       <c r="A483" t="s">
         <v>450</v>
       </c>
@@ -25828,7 +25834,7 @@
         <v>44074</v>
       </c>
     </row>
-    <row r="484" spans="1:14" ht="15">
+    <row r="484" spans="1:14">
       <c r="A484" t="s">
         <v>70</v>
       </c>
@@ -25872,7 +25878,7 @@
         <v>44012</v>
       </c>
     </row>
-    <row r="485" spans="1:14" ht="15">
+    <row r="485" spans="1:14">
       <c r="A485" t="s">
         <v>806</v>
       </c>
@@ -25916,7 +25922,7 @@
         <v>44012</v>
       </c>
     </row>
-    <row r="486" spans="1:14" ht="15">
+    <row r="486" spans="1:14">
       <c r="A486" t="s">
         <v>23</v>
       </c>
@@ -25960,7 +25966,7 @@
         <v>36403</v>
       </c>
     </row>
-    <row r="487" spans="1:14" ht="15">
+    <row r="487" spans="1:14">
       <c r="A487" t="s">
         <v>14</v>
       </c>
@@ -26004,7 +26010,7 @@
         <v>36219</v>
       </c>
     </row>
-    <row r="488" spans="1:14" ht="15">
+    <row r="488" spans="1:14">
       <c r="A488" t="s">
         <v>387</v>
       </c>
@@ -26048,7 +26054,7 @@
         <v>36525</v>
       </c>
     </row>
-    <row r="489" spans="1:14" ht="15">
+    <row r="489" spans="1:14">
       <c r="A489" t="s">
         <v>45</v>
       </c>
@@ -26092,7 +26098,7 @@
         <v>36769</v>
       </c>
     </row>
-    <row r="490" spans="1:14" ht="15">
+    <row r="490" spans="1:14">
       <c r="A490" t="s">
         <v>309</v>
       </c>
@@ -26136,7 +26142,7 @@
         <v>36280</v>
       </c>
     </row>
-    <row r="491" spans="1:14" ht="15">
+    <row r="491" spans="1:14">
       <c r="A491" t="s">
         <v>36</v>
       </c>
@@ -26180,7 +26186,7 @@
         <v>36280</v>
       </c>
     </row>
-    <row r="492" spans="1:14" ht="15">
+    <row r="492" spans="1:14">
       <c r="A492" t="s">
         <v>305</v>
       </c>
@@ -26224,7 +26230,7 @@
         <v>36981</v>
       </c>
     </row>
-    <row r="493" spans="1:14" ht="15">
+    <row r="493" spans="1:14">
       <c r="A493" t="s">
         <v>94</v>
       </c>
@@ -26268,7 +26274,7 @@
         <v>36525</v>
       </c>
     </row>
-    <row r="494" spans="1:14" ht="15">
+    <row r="494" spans="1:14">
       <c r="A494" t="s">
         <v>36</v>
       </c>
@@ -26312,7 +26318,7 @@
         <v>36707</v>
       </c>
     </row>
-    <row r="495" spans="1:14" ht="15">
+    <row r="495" spans="1:14">
       <c r="A495" t="s">
         <v>1329</v>
       </c>
@@ -26356,7 +26362,7 @@
         <v>36891</v>
       </c>
     </row>
-    <row r="496" spans="1:14" ht="15">
+    <row r="496" spans="1:14">
       <c r="A496" t="s">
         <v>45</v>
       </c>
@@ -26400,7 +26406,7 @@
         <v>36219</v>
       </c>
     </row>
-    <row r="497" spans="1:14" ht="15">
+    <row r="497" spans="1:14">
       <c r="A497" t="s">
         <v>1219</v>
       </c>
@@ -26444,7 +26450,7 @@
         <v>36219</v>
       </c>
     </row>
-    <row r="498" spans="1:14" ht="15">
+    <row r="498" spans="1:14">
       <c r="A498" t="s">
         <v>70</v>
       </c>
@@ -26488,7 +26494,7 @@
         <v>36616</v>
       </c>
     </row>
-    <row r="499" spans="1:14" ht="15">
+    <row r="499" spans="1:14">
       <c r="A499" t="s">
         <v>70</v>
       </c>
@@ -26532,7 +26538,7 @@
         <v>36433</v>
       </c>
     </row>
-    <row r="500" spans="1:14" ht="15">
+    <row r="500" spans="1:14">
       <c r="A500" t="s">
         <v>230</v>
       </c>
@@ -26576,7 +26582,7 @@
         <v>36891</v>
       </c>
     </row>
-    <row r="501" spans="1:14" ht="15">
+    <row r="501" spans="1:14">
       <c r="A501" t="s">
         <v>52</v>
       </c>
@@ -26620,7 +26626,7 @@
         <v>36219</v>
       </c>
     </row>
-    <row r="502" spans="1:14" ht="15">
+    <row r="502" spans="1:14">
       <c r="A502" t="s">
         <v>52</v>
       </c>
@@ -26664,7 +26670,7 @@
         <v>36433</v>
       </c>
     </row>
-    <row r="503" spans="1:14" ht="15">
+    <row r="503" spans="1:14">
       <c r="A503" t="s">
         <v>94</v>
       </c>
@@ -26708,7 +26714,7 @@
         <v>36677</v>
       </c>
     </row>
-    <row r="504" spans="1:14" ht="15">
+    <row r="504" spans="1:14">
       <c r="A504" t="s">
         <v>255</v>
       </c>
@@ -26752,7 +26758,7 @@
         <v>36372</v>
       </c>
     </row>
-    <row r="505" spans="1:14" ht="15">
+    <row r="505" spans="1:14">
       <c r="A505" t="s">
         <v>450</v>
       </c>
@@ -26796,7 +26802,7 @@
         <v>36525</v>
       </c>
     </row>
-    <row r="506" spans="1:14" ht="15">
+    <row r="506" spans="1:14">
       <c r="A506" t="s">
         <v>23</v>
       </c>
@@ -26840,7 +26846,7 @@
         <v>37437</v>
       </c>
     </row>
-    <row r="507" spans="1:14" ht="15">
+    <row r="507" spans="1:14">
       <c r="A507" t="s">
         <v>14</v>
       </c>
@@ -26884,7 +26890,7 @@
         <v>36891</v>
       </c>
     </row>
-    <row r="508" spans="1:14" ht="15">
+    <row r="508" spans="1:14">
       <c r="A508" t="s">
         <v>45</v>
       </c>
@@ -26928,7 +26934,7 @@
         <v>36341</v>
       </c>
     </row>
-    <row r="509" spans="1:14" ht="15">
+    <row r="509" spans="1:14">
       <c r="A509" t="s">
         <v>387</v>
       </c>
@@ -26972,7 +26978,7 @@
         <v>36525</v>
       </c>
     </row>
-    <row r="510" spans="1:14" ht="15">
+    <row r="510" spans="1:14">
       <c r="A510" t="s">
         <v>70</v>
       </c>
@@ -27016,7 +27022,7 @@
         <v>36525</v>
       </c>
     </row>
-    <row r="511" spans="1:14" ht="15">
+    <row r="511" spans="1:14">
       <c r="A511" t="s">
         <v>113</v>
       </c>
@@ -27060,7 +27066,7 @@
         <v>36981</v>
       </c>
     </row>
-    <row r="512" spans="1:14" ht="15">
+    <row r="512" spans="1:14">
       <c r="A512" t="s">
         <v>36</v>
       </c>
@@ -27104,7 +27110,7 @@
         <v>37621</v>
       </c>
     </row>
-    <row r="513" spans="1:14" ht="15">
+    <row r="513" spans="1:14">
       <c r="A513" t="s">
         <v>45</v>
       </c>
@@ -27148,7 +27154,7 @@
         <v>36494</v>
       </c>
     </row>
-    <row r="514" spans="1:14" ht="15">
+    <row r="514" spans="1:14">
       <c r="A514" t="s">
         <v>146</v>
       </c>
@@ -27192,7 +27198,7 @@
         <v>36616</v>
       </c>
     </row>
-    <row r="515" spans="1:14" ht="15">
+    <row r="515" spans="1:14">
       <c r="A515" t="s">
         <v>29</v>
       </c>
@@ -27236,7 +27242,7 @@
         <v>37407</v>
       </c>
     </row>
-    <row r="516" spans="1:14" ht="15">
+    <row r="516" spans="1:14">
       <c r="A516" t="s">
         <v>1372</v>
       </c>
@@ -27280,7 +27286,7 @@
         <v>36707</v>
       </c>
     </row>
-    <row r="517" spans="1:14" ht="15">
+    <row r="517" spans="1:14">
       <c r="A517" t="s">
         <v>70</v>
       </c>
@@ -27324,7 +27330,7 @@
         <v>36799</v>
       </c>
     </row>
-    <row r="518" spans="1:14" ht="15">
+    <row r="518" spans="1:14">
       <c r="A518" t="s">
         <v>230</v>
       </c>
@@ -27368,7 +27374,7 @@
         <v>37072</v>
       </c>
     </row>
-    <row r="519" spans="1:14" ht="15">
+    <row r="519" spans="1:14">
       <c r="A519" t="s">
         <v>52</v>
       </c>
@@ -27412,7 +27418,7 @@
         <v>36616</v>
       </c>
     </row>
-    <row r="520" spans="1:14" ht="15">
+    <row r="520" spans="1:14">
       <c r="A520" t="s">
         <v>52</v>
       </c>
@@ -27457,16 +27463,17 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N520" xr:uid="{5D439DCE-415E-CC4E-A606-659E4FA80866}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E07A98-9DBC-9342-9E06-B11E6B087F26}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -27481,8 +27488,13 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>1385</v>
       </c>
     </row>

</xml_diff>